<commit_message>
Update on baccara timeplan
</commit_message>
<xml_diff>
--- a/Dokumentation/ZeitplanBaccara.xlsx
+++ b/Dokumentation/ZeitplanBaccara.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liberatys/Desktop/Projects/Programmierwochen/Casino/Dokumentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49AEE7D6-907E-924A-A080-0DE21B5D3928}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB177C55-7D99-684A-BDBE-9EBB68895F94}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19600" xr2:uid="{86CB73B0-A300-F347-8281-1F427C21E058}"/>
   </bookViews>
@@ -520,7 +520,7 @@
   <dimension ref="B2:S34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>